<commit_message>
Add UC1 wireframe and sylfFirmware
</commit_message>
<xml_diff>
--- a/6.Gerenciamento de Projeto/SYLF - Checklist Verificacao de Projeto.xlsx
+++ b/6.Gerenciamento de Projeto/SYLF - Checklist Verificacao de Projeto.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06C97F0-33D2-4299-97B6-9D11C902B4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="17880" windowHeight="11835" tabRatio="666" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="17880" windowHeight="11835" tabRatio="666" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <sheet name="Ver-Construção1" sheetId="3" r:id="rId5"/>
     <sheet name="Ver-Transição1" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -206,12 +205,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -356,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -375,12 +374,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -492,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -544,12 +543,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -578,7 +577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -661,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -694,7 +693,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -713,7 +712,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="120">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1078,7 +1077,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="17">
     <font>
       <sz val="11"/>
@@ -1474,6 +1473,7 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1525,11 +1525,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1556,7 +1555,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1580,7 +1579,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1716,7 +1715,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1783,7 +1782,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2300,7 +2299,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="165674367"/>
@@ -2359,7 +2358,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="165667647"/>
@@ -2401,12 +2400,13 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2414,7 +2414,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2438,7 +2437,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2452,7 +2451,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2514,7 +2513,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2823,10 +2822,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3031,7 +3030,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1202945552"/>
@@ -3090,7 +3089,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1401041264"/>
@@ -3132,7 +3131,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3162,7 +3161,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3176,7 +3175,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3238,7 +3237,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3779,7 +3778,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1261194848"/>
@@ -3838,7 +3837,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1261193408"/>
@@ -3880,7 +3879,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3910,7 +3909,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3924,7 +3923,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3986,7 +3985,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4551,7 +4550,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1193986912"/>
@@ -4610,7 +4609,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1193985952"/>
@@ -4652,7 +4651,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4682,7 +4681,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7317,7 +7316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7331,10 +7330,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="18" t="s">
@@ -7357,9 +7356,9 @@
       <c r="A4" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="20" t="e">
+      <c r="B4" s="20">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7393,7 +7392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6B2C1B-A599-4159-99C1-DE703E343043}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -7467,21 +7466,21 @@
       <c r="N2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="25" t="e">
+      <c r="O2" s="25">
         <f>('Ver-Elaboração1'!$G$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P2" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="P2" s="25">
         <f>('Ver-Elaboração1'!$H$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q2" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="25">
         <f>('Ver-Elaboração1'!$I$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R2" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="R2" s="25">
         <f>('Ver-Elaboração1'!$J$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7507,21 +7506,21 @@
       <c r="N3" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="25" t="e">
+      <c r="O3" s="25">
         <f>('Ver-Elaboração1'!$G$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P3" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="P3" s="25">
         <f>('Ver-Elaboração1'!$H$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q3" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="25">
         <f>('Ver-Elaboração1'!$I$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R3" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="R3" s="25">
         <f>('Ver-Elaboração1'!$J$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -8431,11 +8430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8453,41 +8452,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
         <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -8510,7 +8509,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9"/>
@@ -8538,7 +8537,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="35"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -8552,7 +8551,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="9"/>
@@ -8580,7 +8579,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="22">
         <v>2</v>
       </c>
@@ -8594,7 +8593,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="5">
         <v>3</v>
       </c>
@@ -8608,7 +8607,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="15">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5">
         <v>4</v>
       </c>
@@ -8622,7 +8621,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="15">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5">
         <v>5</v>
       </c>
@@ -8636,7 +8635,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5">
         <v>6</v>
       </c>
@@ -8650,7 +8649,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>3</v>
@@ -8676,7 +8675,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="23">
         <v>7</v>
       </c>
@@ -8690,7 +8689,7 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="5">
         <v>8</v>
       </c>
@@ -8704,7 +8703,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>9</v>
       </c>
@@ -8718,7 +8717,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A17" s="31"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="23">
         <v>10</v>
       </c>
@@ -8732,7 +8731,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="15">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>11</v>
       </c>
@@ -8746,7 +8745,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
         <v>97</v>
@@ -8772,7 +8771,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="23">
         <v>12</v>
       </c>
@@ -8786,7 +8785,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="30">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>13</v>
       </c>
@@ -8800,7 +8799,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="31"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
         <v>4</v>
@@ -8826,7 +8825,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="30">
-      <c r="A23" s="31"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="23">
         <v>14</v>
       </c>
@@ -8840,7 +8839,7 @@
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -8854,7 +8853,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="31"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
         <v>36</v>
@@ -8880,7 +8879,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="30">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="23">
         <v>16</v>
       </c>
@@ -8894,7 +8893,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>17</v>
       </c>
@@ -8908,7 +8907,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="31"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
         <v>13</v>
@@ -8934,7 +8933,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="31"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="23">
         <v>21</v>
       </c>
@@ -8948,7 +8947,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="31"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="5">
         <v>22</v>
       </c>
@@ -8962,7 +8961,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="31"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="5">
         <v>23</v>
       </c>
@@ -8976,7 +8975,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="31"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="5">
         <v>24</v>
       </c>
@@ -8990,7 +8989,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="31"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="5">
         <v>25</v>
       </c>
@@ -9004,7 +9003,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="30">
-      <c r="A34" s="31"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="5">
         <v>26</v>
       </c>
@@ -9017,7 +9016,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A35" s="31"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="5">
         <v>27</v>
       </c>
@@ -9031,7 +9030,7 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="31"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="5">
         <v>28</v>
       </c>
@@ -9045,7 +9044,7 @@
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="9"/>
@@ -9073,7 +9072,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="23">
         <v>30</v>
       </c>
@@ -9087,7 +9086,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="30">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5">
         <v>31</v>
       </c>
@@ -9105,7 +9104,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5">
         <v>32</v>
       </c>
@@ -9119,7 +9118,7 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:10" ht="39" customHeight="1">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -9145,7 +9144,7 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36" xr:uid="{3299DAEA-DE76-409E-BA4B-99D6162A5554}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9156,11 +9155,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9175,45 +9174,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="45">
+      <c r="B2" s="34"/>
+      <c r="C2" s="28">
         <v>45878</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="21" t="e">
+      <c r="E2" s="41"/>
+      <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -9236,7 +9235,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -9248,14 +9247,16 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
@@ -9268,7 +9269,7 @@
       </c>
       <c r="I6">
         <f>COUNTIF(D6,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f>COUNTIF(D6,"NA")</f>
@@ -9276,7 +9277,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -9286,14 +9287,16 @@
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
@@ -9306,7 +9309,7 @@
       </c>
       <c r="I8">
         <f>COUNTIF(D8,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f>COUNTIF(D8,"NA")</f>
@@ -9314,7 +9317,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="5">
         <v>3</v>
       </c>
@@ -9330,7 +9333,7 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" ht="15">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
         <v>97</v>
@@ -9340,7 +9343,7 @@
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="23">
         <v>4</v>
       </c>
@@ -9368,7 +9371,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="23">
         <v>5</v>
       </c>
@@ -9380,7 +9383,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="5">
         <v>6</v>
       </c>
@@ -9392,7 +9395,7 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5">
         <v>7</v>
       </c>
@@ -9404,7 +9407,7 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>4</v>
@@ -9414,7 +9417,7 @@
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -9442,7 +9445,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="9"/>
@@ -9454,7 +9457,7 @@
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -9482,7 +9485,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="30">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="23">
         <v>10</v>
       </c>
@@ -9494,7 +9497,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -9506,7 +9509,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="45">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>12</v>
       </c>
@@ -9518,7 +9521,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="35" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="9"/>
@@ -9530,7 +9533,7 @@
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="30">
-      <c r="A23" s="31"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="5">
         <v>17</v>
       </c>
@@ -9558,7 +9561,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5">
         <v>18</v>
       </c>
@@ -9570,7 +9573,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="31"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="5">
         <v>19</v>
       </c>
@@ -9582,7 +9585,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="5">
         <v>21</v>
       </c>
@@ -9594,7 +9597,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>22</v>
       </c>
@@ -9606,7 +9609,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="9"/>
@@ -9618,7 +9621,7 @@
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="41"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="5">
         <v>23</v>
       </c>
@@ -9646,7 +9649,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="41"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="5">
         <v>24</v>
       </c>
@@ -9658,7 +9661,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:10" ht="30">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="5">
         <v>25</v>
       </c>
@@ -9670,7 +9673,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="5">
         <v>26</v>
       </c>
@@ -9682,7 +9685,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="5">
         <v>27</v>
       </c>
@@ -9694,7 +9697,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="5">
         <v>28</v>
       </c>
@@ -9706,7 +9709,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
@@ -9718,7 +9721,7 @@
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="30">
-      <c r="A36" s="30"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5">
         <v>29</v>
       </c>
@@ -9746,7 +9749,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5">
         <v>30</v>
       </c>
@@ -9758,7 +9761,7 @@
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5">
         <v>31</v>
       </c>
@@ -9770,7 +9773,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="15">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
         <v>15</v>
@@ -9780,7 +9783,7 @@
       <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5">
         <v>32</v>
       </c>
@@ -9808,7 +9811,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -9833,10 +9836,10 @@
     <mergeCell ref="A5:A16"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17 D22 D28 D35 D39" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17 D22 D28 D35 D39">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D40:D41 D36:D38 D29:D34 D18:D21 D16 D11:D14 D8:D9 D6 D23:D27" xr:uid="{08EF66E2-96BC-4443-A5E2-B5C56733D826}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D40:D41 D36:D38 D29:D34 D18:D21 D16 D11:D14 D8:D9 D6 D23:D27">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9846,7 +9849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9865,41 +9868,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D42,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -9922,7 +9925,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -9934,7 +9937,7 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -9962,7 +9965,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -9972,7 +9975,7 @@
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -10000,7 +10003,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
         <v>97</v>
@@ -10010,7 +10013,7 @@
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -10038,7 +10041,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -10050,7 +10053,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -10062,7 +10065,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>4</v>
@@ -10072,7 +10075,7 @@
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5">
         <v>6</v>
       </c>
@@ -10100,7 +10103,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="9"/>
@@ -10112,7 +10115,7 @@
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>8</v>
       </c>
@@ -10140,7 +10143,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="9"/>
@@ -10152,7 +10155,7 @@
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="15">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>11</v>
       </c>
@@ -10180,7 +10183,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="30">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5">
         <v>13</v>
       </c>
@@ -10192,7 +10195,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5">
         <v>14</v>
       </c>
@@ -10204,7 +10207,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>15</v>
       </c>
@@ -10216,7 +10219,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="31"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="5">
         <v>16</v>
       </c>
@@ -10228,7 +10231,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="35" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="9"/>
@@ -10240,7 +10243,7 @@
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="23">
         <v>17</v>
       </c>
@@ -10268,7 +10271,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="31"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="5">
         <v>18</v>
       </c>
@@ -10280,7 +10283,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="5">
         <v>19</v>
       </c>
@@ -10292,7 +10295,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>21</v>
       </c>
@@ -10304,7 +10307,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="31"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="5">
         <v>22</v>
       </c>
@@ -10316,7 +10319,7 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="9"/>
@@ -10328,7 +10331,7 @@
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="41"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="5">
         <v>24</v>
       </c>
@@ -10356,7 +10359,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="30">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="5">
         <v>26</v>
       </c>
@@ -10368,7 +10371,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="5">
         <v>27</v>
       </c>
@@ -10380,7 +10383,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="5">
         <v>28</v>
       </c>
@@ -10392,7 +10395,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="5">
         <v>29</v>
       </c>
@@ -10404,7 +10407,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
@@ -10416,7 +10419,7 @@
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="30">
-      <c r="A36" s="30"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5">
         <v>30</v>
       </c>
@@ -10444,7 +10447,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5">
         <v>31</v>
       </c>
@@ -10456,7 +10459,7 @@
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5">
         <v>32</v>
       </c>
@@ -10468,7 +10471,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="15">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5"/>
       <c r="C39" s="8" t="s">
         <v>105</v>
@@ -10478,7 +10481,7 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
         <v>15</v>
@@ -10488,7 +10491,7 @@
       <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -10516,7 +10519,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15">
-      <c r="A42" s="30"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="5">
         <v>34</v>
       </c>
@@ -10557,23 +10560,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D36:D39 D41:D42 D18:D22 D24:D28 D30:D34" xr:uid="{2F69EF16-DBD3-468C-8391-039EC6576FAB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D36:D39 D41:D42 D18:D22 D24:D28 D30:D34">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10583,7 +10586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10602,41 +10605,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D43,"Sim")/(COUNTA(D5:D43)-COUNTIF(D5:D43,"NA"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -10659,7 +10662,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -10671,7 +10674,7 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -10699,7 +10702,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -10709,7 +10712,7 @@
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -10737,7 +10740,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
         <v>14</v>
@@ -10747,7 +10750,7 @@
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -10775,7 +10778,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -10787,7 +10790,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -10799,7 +10802,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>4</v>
@@ -10809,7 +10812,7 @@
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5">
         <v>6</v>
       </c>
@@ -10837,7 +10840,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="9"/>
@@ -10849,7 +10852,7 @@
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>8</v>
       </c>
@@ -10877,7 +10880,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="9"/>
@@ -10889,7 +10892,7 @@
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -10917,7 +10920,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -10929,7 +10932,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -10941,7 +10944,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="35"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="5">
         <v>13</v>
       </c>
@@ -10953,7 +10956,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="35" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="9"/>
@@ -10965,7 +10968,7 @@
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="31"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="5">
         <v>14</v>
       </c>
@@ -10993,7 +10996,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -11005,7 +11008,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="9"/>
@@ -11017,7 +11020,7 @@
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="23">
         <v>24</v>
       </c>
@@ -11045,7 +11048,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="1" customFormat="1" ht="45">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>25</v>
       </c>
@@ -11057,7 +11060,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="31"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
         <v>10</v>
@@ -11067,7 +11070,7 @@
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="31"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="23">
         <v>26</v>
       </c>
@@ -11095,7 +11098,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="9"/>
@@ -11107,7 +11110,7 @@
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="5">
         <v>19</v>
       </c>
@@ -11135,7 +11138,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="30">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="5">
         <v>20</v>
       </c>
@@ -11147,7 +11150,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="5">
         <v>21</v>
       </c>
@@ -11159,7 +11162,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="5">
         <v>24</v>
       </c>
@@ -11171,7 +11174,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="41"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="5">
         <v>25</v>
       </c>
@@ -11183,7 +11186,7 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="9"/>
@@ -11195,7 +11198,7 @@
       <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:10" ht="30">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5">
         <v>26</v>
       </c>
@@ -11223,7 +11226,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5">
         <v>27</v>
       </c>
@@ -11235,7 +11238,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="30">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5">
         <v>28</v>
       </c>
@@ -11247,7 +11250,7 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5"/>
       <c r="C40" s="8" t="s">
         <v>105</v>
@@ -11257,7 +11260,7 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
         <v>15</v>
@@ -11267,7 +11270,7 @@
       <c r="F41" s="12"/>
     </row>
     <row r="42" spans="1:10" ht="15">
-      <c r="A42" s="30"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="5">
         <v>29</v>
       </c>
@@ -11295,7 +11298,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15">
-      <c r="A43" s="30"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="5">
         <v>30</v>
       </c>
@@ -11336,11 +11339,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A25:A29"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:F1"/>
@@ -11348,12 +11346,17 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D23:D24 D26:D27 D29 D31:D35 D42:D43 D18:D21 D37:D40" xr:uid="{A5BD53E1-86A3-4B0D-8790-16FF9D054B9C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D23:D24 D26:D27 D29 D31:D35 D42:D43 D18:D21 D37:D40">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Atualizar nomeação de artefatos e checklist do projeto.
</commit_message>
<xml_diff>
--- a/6.Gerenciamento de Projeto/SYLF - Checklist Verificacao de Projeto.xlsx
+++ b/6.Gerenciamento de Projeto/SYLF - Checklist Verificacao de Projeto.xlsx
@@ -712,7 +712,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="121">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1065,13 +1065,16 @@
     <t>Não</t>
   </si>
   <si>
-    <t>Não está subido todos os artefatos ao repositório ainda.</t>
-  </si>
-  <si>
-    <t>Completar a subida dos artefatos logo em breve.</t>
-  </si>
-  <si>
     <t>Brian Kofi Agyei Wealth</t>
+  </si>
+  <si>
+    <t>Parcialmente</t>
+  </si>
+  <si>
+    <t>Não houve nenhuma mudança.</t>
+  </si>
+  <si>
+    <t>Necessitou do termino do diagrama de arquitetura.</t>
   </si>
 </sst>
 </file>
@@ -1633,10 +1636,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.81818181818181823</c:v>
+                  <c:v>0.90909090909090906</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.35714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1892,7 +1895,7 @@
                   <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2118,7 +2121,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2602,7 +2605,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2617,13 +2620,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2715,7 +2718,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2724,13 +2727,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2831,28 +2834,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7349,7 +7352,7 @@
       </c>
       <c r="B3" s="20">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.81818181818181823</v>
+        <v>0.90909090909090906</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7358,7 +7361,7 @@
       </c>
       <c r="B4" s="20">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7546,21 +7549,21 @@
       <c r="N4" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="25" t="e">
+      <c r="O4" s="25">
         <f>('Ver-Elaboração1'!$G$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="25" t="e">
+        <v>0.75</v>
+      </c>
+      <c r="P4" s="25">
         <f>('Ver-Elaboração1'!$H$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q4" s="25" t="e">
+        <v>0.25</v>
+      </c>
+      <c r="Q4" s="25">
         <f>('Ver-Elaboração1'!$I$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R4" s="25">
         <f>('Ver-Elaboração1'!$J$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -7586,21 +7589,21 @@
       <c r="N5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="25" t="e">
+      <c r="O5" s="25">
         <f>('Ver-Elaboração1'!$G$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="P5" s="25">
         <f>('Ver-Elaboração1'!$H$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q5" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="25">
         <f>('Ver-Elaboração1'!$I$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="R5" s="25">
         <f>('Ver-Elaboração1'!$J$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -7666,21 +7669,21 @@
       <c r="N7" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="25" t="e">
+      <c r="O7" s="25">
         <f>('Ver-Elaboração1'!$G$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="P7" s="25">
         <f>('Ver-Elaboração1'!$H$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="25" t="e">
+        <v>0.75</v>
+      </c>
+      <c r="Q7" s="25">
         <f>('Ver-Elaboração1'!$I$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="25" t="e">
+        <v>0.25</v>
+      </c>
+      <c r="R7" s="25">
         <f>('Ver-Elaboração1'!$J$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -7746,21 +7749,21 @@
       <c r="N9" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="25" t="e">
+      <c r="O9" s="25">
         <f>('Ver-Elaboração1'!$G$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="25" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="P9" s="25">
         <f>('Ver-Elaboração1'!$H$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="25" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="Q9" s="25">
         <f>('Ver-Elaboração1'!$I$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="25" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="R9" s="25">
         <f>('Ver-Elaboração1'!$J$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -7786,21 +7789,21 @@
       <c r="N10" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="25" t="e">
+      <c r="O10" s="25">
         <f>('Ver-Elaboração1'!$G$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="25" t="e">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P10" s="25">
         <f>('Ver-Elaboração1'!$H$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="25">
         <f>('Ver-Elaboração1'!$I$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="25" t="e">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="R10" s="25">
         <f>('Ver-Elaboração1'!$J$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -7809,7 +7812,7 @@
       </c>
       <c r="B11" s="25">
         <f>('Ver-Iniciação1'!$G$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="C11" s="25">
         <f>('Ver-Iniciação1'!$H$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
@@ -7817,7 +7820,7 @@
       </c>
       <c r="D11" s="25">
         <f>('Ver-Iniciação1'!$I$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="E11" s="25">
         <f>('Ver-Iniciação1'!$J$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
@@ -7826,21 +7829,21 @@
       <c r="N11" t="s">
         <v>56</v>
       </c>
-      <c r="O11" s="25" t="e">
+      <c r="O11" s="25">
         <f>('Ver-Elaboração1'!$G$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="P11" s="25">
         <f>('Ver-Elaboração1'!$H$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="25">
         <f>('Ver-Elaboração1'!$I$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R11" s="25">
         <f>('Ver-Elaboração1'!$J$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -7866,21 +7869,21 @@
       <c r="N12" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="25" t="e">
+      <c r="O12" s="25">
         <f>('Ver-Elaboração1'!$G$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="P12" s="25">
         <f>('Ver-Elaboração1'!$H$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="25">
         <f>('Ver-Elaboração1'!$I$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="R12" s="25">
         <f>('Ver-Elaboração1'!$J$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -8433,8 +8436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8473,7 +8476,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.81818181818181823</v>
+        <v>0.90909090909090906</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -9056,7 +9059,7 @@
       <c r="F37" s="12"/>
       <c r="G37">
         <f>COUNTIF(D38:D41,"Sim")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H37">
         <f>COUNTIF(D38:D41,"Parcialmente")</f>
@@ -9064,7 +9067,7 @@
       </c>
       <c r="I37">
         <f>COUNTIF(D38:D41,"Não")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J37">
         <f>COUNTIF(D38:D41,"NA")</f>
@@ -9094,14 +9097,10 @@
         <v>38</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>118</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:10" ht="15">
       <c r="A40" s="31"/>
@@ -9112,7 +9111,7 @@
         <v>39</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -9158,8 +9157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9197,7 +9196,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -9206,7 +9205,7 @@
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>43</v>
@@ -9246,7 +9245,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="32"/>
       <c r="B6" s="5">
         <v>1</v>
@@ -9257,7 +9256,9 @@
       <c r="D6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="F6" s="8"/>
       <c r="G6">
         <f>COUNTIF(D6,"Sim")</f>
@@ -9324,7 +9325,9 @@
       <c r="C9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9"/>
@@ -9350,16 +9353,18 @@
       <c r="C11" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11">
         <f>COUNTIF(D11:D14,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <f>COUNTIF(D11:D14,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f>COUNTIF(D11:D14,"Não")</f>
@@ -9378,7 +9383,9 @@
       <c r="C12" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -9390,8 +9397,12 @@
       <c r="C13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="30">
@@ -9402,7 +9413,9 @@
       <c r="C14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
@@ -9424,7 +9437,9 @@
       <c r="C16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
@@ -9437,7 +9452,7 @@
       </c>
       <c r="I16">
         <f>COUNTIF(D16,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <f>COUNTIF(D16,"NA")</f>
@@ -9464,7 +9479,9 @@
       <c r="C18" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18">
@@ -9473,11 +9490,11 @@
       </c>
       <c r="H18">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I18">
         <f>COUNTIF(D18:D21,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <f>COUNTIF(D18:D21,"NA")</f>
@@ -9492,7 +9509,9 @@
       <c r="C19" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
@@ -9504,7 +9523,9 @@
       <c r="C20" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -9516,7 +9537,9 @@
       <c r="C21" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -9540,20 +9563,22 @@
       <c r="C23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23">
         <f>COUNTIF(D23:D27,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <f>COUNTIF(D23:D27,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <f>COUNTIF(D23:D27,"Não")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23">
         <f>COUNTIF(D23:D27,"NA")</f>
@@ -9568,7 +9593,9 @@
       <c r="C24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
@@ -9580,7 +9607,9 @@
       <c r="C25" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
@@ -9592,7 +9621,9 @@
       <c r="C26" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
@@ -9604,7 +9635,9 @@
       <c r="C27" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
@@ -9628,12 +9661,14 @@
       <c r="C29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29">
         <f>COUNTIF(D29:D34,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <f>COUNTIF(D29:D34,"Parcialmente")</f>
@@ -9641,7 +9676,7 @@
       </c>
       <c r="I29">
         <f>COUNTIF(D29:D34,"Não")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J29">
         <f>COUNTIF(D29:D34,"NA")</f>
@@ -9656,7 +9691,9 @@
       <c r="C30" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
@@ -9668,7 +9705,9 @@
       <c r="C31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -9680,7 +9719,9 @@
       <c r="C32" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
@@ -9692,7 +9733,9 @@
       <c r="C33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
@@ -9704,7 +9747,9 @@
       <c r="C34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -9728,12 +9773,14 @@
       <c r="C36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36">
         <f>COUNTIF(D36:D38,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36">
         <f>COUNTIF(D36:D38,"Parcialmente")</f>
@@ -9756,7 +9803,9 @@
       <c r="C37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
@@ -9768,7 +9817,9 @@
       <c r="C38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -9790,7 +9841,9 @@
       <c r="C40" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40">
@@ -9803,7 +9856,7 @@
       </c>
       <c r="I40">
         <f>COUNTIF(D40:D41,"Não")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J40">
         <f>COUNTIF(D40:D41,"NA")</f>
@@ -9818,7 +9871,9 @@
       <c r="C41" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
@@ -9844,7 +9899,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9852,7 +9908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>